<commit_message>
Indicator visualization - JP
</commit_message>
<xml_diff>
--- a/data/July-Sep 2022/Reproductive maternal/Reproductive Health monthly prov.xlsx
+++ b/data/July-Sep 2022/Reproductive maternal/Reproductive Health monthly prov.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan.killian\Documents\Zambia E4 Health\data\July-Sep 2022\Reproductive maternal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JACK.PAYNE\Documents\Zambia-E4H\data\July-Sep 2022\Reproductive maternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB6CBD32-1EFE-4489-B644-F31421AC93A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DF5A23-68A1-48D4-9FB1-674E7C6E3718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reproductive Health Monthly dat" sheetId="1" r:id="rId1"/>
     <sheet name="export" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="53">
   <si>
     <t>periodname</t>
   </si>
@@ -160,11 +173,32 @@
   <si>
     <t>mat_dths</t>
   </si>
+  <si>
+    <t>neo_dths</t>
+  </si>
+  <si>
+    <t>anc_1st</t>
+  </si>
+  <si>
+    <t>anc_all</t>
+  </si>
+  <si>
+    <t>anc_1st_und20</t>
+  </si>
+  <si>
+    <t>folic</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>anc_highrisk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1006,21 +1040,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" customWidth="1"/>
-    <col min="10" max="19" width="17.88671875" customWidth="1"/>
+    <col min="3" max="8" width="17.90625" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" customWidth="1"/>
+    <col min="10" max="19" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44947</v>
       </c>
@@ -1138,7 +1172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44947</v>
       </c>
@@ -1197,7 +1231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44947</v>
       </c>
@@ -1250,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44947</v>
       </c>
@@ -1309,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44947</v>
       </c>
@@ -1365,7 +1399,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44947</v>
       </c>
@@ -1424,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44947</v>
       </c>
@@ -1483,7 +1517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44947</v>
       </c>
@@ -1542,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44947</v>
       </c>
@@ -1595,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44947</v>
       </c>
@@ -1654,7 +1688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44978</v>
       </c>
@@ -1713,7 +1747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44978</v>
       </c>
@@ -1772,7 +1806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44978</v>
       </c>
@@ -1831,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44978</v>
       </c>
@@ -1890,7 +1924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44978</v>
       </c>
@@ -1949,7 +1983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44978</v>
       </c>
@@ -2008,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44978</v>
       </c>
@@ -2067,7 +2101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44978</v>
       </c>
@@ -2126,7 +2160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44978</v>
       </c>
@@ -2185,7 +2219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44978</v>
       </c>
@@ -2244,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45006</v>
       </c>
@@ -2303,7 +2337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45006</v>
       </c>
@@ -2362,7 +2396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45006</v>
       </c>
@@ -2421,7 +2455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45006</v>
       </c>
@@ -2477,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45006</v>
       </c>
@@ -2533,7 +2567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45006</v>
       </c>
@@ -2592,7 +2626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45006</v>
       </c>
@@ -2651,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45006</v>
       </c>
@@ -2710,7 +2744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45006</v>
       </c>
@@ -2769,7 +2803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45006</v>
       </c>
@@ -2819,7 +2853,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45037</v>
       </c>
@@ -2878,7 +2912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45037</v>
       </c>
@@ -2937,7 +2971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45037</v>
       </c>
@@ -2996,7 +3030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45037</v>
       </c>
@@ -3052,7 +3086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45037</v>
       </c>
@@ -3108,7 +3142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>45037</v>
       </c>
@@ -3158,7 +3192,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45037</v>
       </c>
@@ -3217,7 +3251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45037</v>
       </c>
@@ -3276,7 +3310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45037</v>
       </c>
@@ -3335,7 +3369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>45037</v>
       </c>
@@ -3394,7 +3428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45067</v>
       </c>
@@ -3453,7 +3487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>45067</v>
       </c>
@@ -3512,7 +3546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45067</v>
       </c>
@@ -3571,7 +3605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45067</v>
       </c>
@@ -3630,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45067</v>
       </c>
@@ -3689,7 +3723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45067</v>
       </c>
@@ -3748,7 +3782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45067</v>
       </c>
@@ -3807,7 +3841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>45067</v>
       </c>
@@ -3866,7 +3900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>45067</v>
       </c>
@@ -3925,7 +3959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>45067</v>
       </c>
@@ -3984,7 +4018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>45098</v>
       </c>
@@ -4043,7 +4077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>45098</v>
       </c>
@@ -4102,7 +4136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>45098</v>
       </c>
@@ -4161,7 +4195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>45098</v>
       </c>
@@ -4217,7 +4251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>45098</v>
       </c>
@@ -4276,7 +4310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>45098</v>
       </c>
@@ -4332,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>45098</v>
       </c>
@@ -4391,7 +4425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>45098</v>
       </c>
@@ -4450,7 +4484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>45098</v>
       </c>
@@ -4509,7 +4543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>45098</v>
       </c>
@@ -4568,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>45128</v>
       </c>
@@ -4627,7 +4661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>45128</v>
       </c>
@@ -4686,7 +4720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>45128</v>
       </c>
@@ -4745,7 +4779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>45128</v>
       </c>
@@ -4801,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>45128</v>
       </c>
@@ -4860,7 +4894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>45128</v>
       </c>
@@ -4919,7 +4953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>45128</v>
       </c>
@@ -4978,7 +5012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>45128</v>
       </c>
@@ -5034,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>45128</v>
       </c>
@@ -5093,7 +5127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>45128</v>
       </c>
@@ -5152,7 +5186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>45159</v>
       </c>
@@ -5211,7 +5245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>45159</v>
       </c>
@@ -5270,7 +5304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>45159</v>
       </c>
@@ -5329,7 +5363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>45159</v>
       </c>
@@ -5379,7 +5413,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>45159</v>
       </c>
@@ -5438,7 +5472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>45159</v>
       </c>
@@ -5497,7 +5531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>45159</v>
       </c>
@@ -5556,7 +5590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>45159</v>
       </c>
@@ -5615,7 +5649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>45159</v>
       </c>
@@ -5674,7 +5708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>45159</v>
       </c>
@@ -5733,7 +5767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>45190</v>
       </c>
@@ -5792,7 +5826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>45190</v>
       </c>
@@ -5851,7 +5885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>45190</v>
       </c>
@@ -5910,7 +5944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>45190</v>
       </c>
@@ -5969,7 +6003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>45190</v>
       </c>
@@ -6028,7 +6062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>45190</v>
       </c>
@@ -6087,7 +6121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>45190</v>
       </c>
@@ -6146,7 +6180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>45190</v>
       </c>
@@ -6205,7 +6239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>45190</v>
       </c>
@@ -6264,7 +6298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>45190</v>
       </c>
@@ -6323,7 +6357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>45220</v>
       </c>
@@ -6382,7 +6416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>45220</v>
       </c>
@@ -6441,7 +6475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>45220</v>
       </c>
@@ -6500,7 +6534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>45220</v>
       </c>
@@ -6559,7 +6593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>45220</v>
       </c>
@@ -6615,7 +6649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>45220</v>
       </c>
@@ -6674,7 +6708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>45220</v>
       </c>
@@ -6733,7 +6767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>45220</v>
       </c>
@@ -6792,7 +6826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>45220</v>
       </c>
@@ -6851,7 +6885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>45220</v>
       </c>
@@ -6910,7 +6944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>45251</v>
       </c>
@@ -6969,7 +7003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>45251</v>
       </c>
@@ -7028,7 +7062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>45251</v>
       </c>
@@ -7087,7 +7121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>45251</v>
       </c>
@@ -7146,7 +7180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>45251</v>
       </c>
@@ -7205,7 +7239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>45251</v>
       </c>
@@ -7264,7 +7298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>45251</v>
       </c>
@@ -7323,7 +7357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>45251</v>
       </c>
@@ -7379,7 +7413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>45251</v>
       </c>
@@ -7438,7 +7472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>45251</v>
       </c>
@@ -7497,7 +7531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>45281</v>
       </c>
@@ -7556,7 +7590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>45281</v>
       </c>
@@ -7615,7 +7649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>45281</v>
       </c>
@@ -7674,7 +7708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>45281</v>
       </c>
@@ -7730,7 +7764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>45281</v>
       </c>
@@ -7789,7 +7823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>45281</v>
       </c>
@@ -7848,7 +7882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>45281</v>
       </c>
@@ -7907,7 +7941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>45281</v>
       </c>
@@ -7966,7 +8000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>45281</v>
       </c>
@@ -8025,7 +8059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>45281</v>
       </c>
@@ -8084,7 +8118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2021</v>
       </c>
@@ -8143,7 +8177,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -8202,7 +8236,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2021</v>
       </c>
@@ -8261,7 +8295,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2021</v>
       </c>
@@ -8320,7 +8354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2021</v>
       </c>
@@ -8379,7 +8413,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2021</v>
       </c>
@@ -8438,7 +8472,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2021</v>
       </c>
@@ -8497,7 +8531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2021</v>
       </c>
@@ -8556,7 +8590,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2021</v>
       </c>
@@ -8615,7 +8649,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -8680,23 +8714,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H106" workbookViewId="0">
-      <selection activeCell="M113" sqref="M113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.21875"/>
-    <col min="3" max="3" width="9.5546875" style="3" customWidth="1"/>
-    <col min="5" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1"/>
-    <col min="12" max="21" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875"/>
+    <col min="3" max="3" width="9.54296875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="17.90625" customWidth="1"/>
+    <col min="7" max="7" width="28.54296875" customWidth="1"/>
+    <col min="8" max="8" width="28.453125" customWidth="1"/>
+    <col min="9" max="10" width="17.90625" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" customWidth="1"/>
+    <col min="12" max="21" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8761,7 +8798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8775,22 +8812,22 @@
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -8814,7 +8851,7 @@
         <v>14</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>16</v>
@@ -8826,7 +8863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44947</v>
       </c>
@@ -8891,7 +8928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44947</v>
       </c>
@@ -8956,7 +8993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44947</v>
       </c>
@@ -9015,7 +9052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44947</v>
       </c>
@@ -9080,7 +9117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44947</v>
       </c>
@@ -9142,7 +9179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44947</v>
       </c>
@@ -9207,7 +9244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44947</v>
       </c>
@@ -9272,7 +9309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44947</v>
       </c>
@@ -9337,7 +9374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44947</v>
       </c>
@@ -9396,7 +9433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44947</v>
       </c>
@@ -9461,7 +9498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44978</v>
       </c>
@@ -9526,7 +9563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44978</v>
       </c>
@@ -9591,7 +9628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44978</v>
       </c>
@@ -9656,7 +9693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44978</v>
       </c>
@@ -9721,7 +9758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44978</v>
       </c>
@@ -9786,7 +9823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44978</v>
       </c>
@@ -9851,7 +9888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44978</v>
       </c>
@@ -9916,7 +9953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44978</v>
       </c>
@@ -9981,7 +10018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44978</v>
       </c>
@@ -10046,7 +10083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44978</v>
       </c>
@@ -10111,7 +10148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45006</v>
       </c>
@@ -10176,7 +10213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45006</v>
       </c>
@@ -10241,7 +10278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45006</v>
       </c>
@@ -10306,7 +10343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45006</v>
       </c>
@@ -10368,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45006</v>
       </c>
@@ -10430,7 +10467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45006</v>
       </c>
@@ -10495,7 +10532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45006</v>
       </c>
@@ -10560,7 +10597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45006</v>
       </c>
@@ -10625,7 +10662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45006</v>
       </c>
@@ -10690,7 +10727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45006</v>
       </c>
@@ -10746,7 +10783,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45037</v>
       </c>
@@ -10811,7 +10848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45037</v>
       </c>
@@ -10876,7 +10913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45037</v>
       </c>
@@ -10941,7 +10978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45037</v>
       </c>
@@ -11003,7 +11040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>45037</v>
       </c>
@@ -11065,7 +11102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45037</v>
       </c>
@@ -11121,7 +11158,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45037</v>
       </c>
@@ -11186,7 +11223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45037</v>
       </c>
@@ -11251,7 +11288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>45037</v>
       </c>
@@ -11316,7 +11353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45037</v>
       </c>
@@ -11381,7 +11418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>45067</v>
       </c>
@@ -11446,7 +11483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45067</v>
       </c>
@@ -11511,7 +11548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45067</v>
       </c>
@@ -11576,7 +11613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45067</v>
       </c>
@@ -11641,7 +11678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45067</v>
       </c>
@@ -11706,7 +11743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45067</v>
       </c>
@@ -11771,7 +11808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>45067</v>
       </c>
@@ -11836,7 +11873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>45067</v>
       </c>
@@ -11901,7 +11938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>45067</v>
       </c>
@@ -11966,7 +12003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>45067</v>
       </c>
@@ -12031,7 +12068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>45098</v>
       </c>
@@ -12096,7 +12133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>45098</v>
       </c>
@@ -12161,7 +12198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>45098</v>
       </c>
@@ -12226,7 +12263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>45098</v>
       </c>
@@ -12288,7 +12325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>45098</v>
       </c>
@@ -12353,7 +12390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>45098</v>
       </c>
@@ -12415,7 +12452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>45098</v>
       </c>
@@ -12480,7 +12517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>45098</v>
       </c>
@@ -12545,7 +12582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>45098</v>
       </c>
@@ -12610,7 +12647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>45098</v>
       </c>
@@ -12675,7 +12712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>45128</v>
       </c>
@@ -12740,7 +12777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>45128</v>
       </c>
@@ -12805,7 +12842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>45128</v>
       </c>
@@ -12870,7 +12907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>45128</v>
       </c>
@@ -12932,7 +12969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>45128</v>
       </c>
@@ -12997,7 +13034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>45128</v>
       </c>
@@ -13062,7 +13099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>45128</v>
       </c>
@@ -13127,7 +13164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>45128</v>
       </c>
@@ -13189,7 +13226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>45128</v>
       </c>
@@ -13254,7 +13291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>45128</v>
       </c>
@@ -13319,7 +13356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>45159</v>
       </c>
@@ -13384,7 +13421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>45159</v>
       </c>
@@ -13449,7 +13486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>45159</v>
       </c>
@@ -13514,7 +13551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>45159</v>
       </c>
@@ -13570,7 +13607,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>45159</v>
       </c>
@@ -13635,7 +13672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>45159</v>
       </c>
@@ -13700,7 +13737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>45159</v>
       </c>
@@ -13765,7 +13802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>45159</v>
       </c>
@@ -13830,7 +13867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>45159</v>
       </c>
@@ -13895,7 +13932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>45159</v>
       </c>
@@ -13960,7 +13997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>45190</v>
       </c>
@@ -14025,7 +14062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>45190</v>
       </c>
@@ -14090,7 +14127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>45190</v>
       </c>
@@ -14155,7 +14192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>45190</v>
       </c>
@@ -14220,7 +14257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>45190</v>
       </c>
@@ -14285,7 +14322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>45190</v>
       </c>
@@ -14350,7 +14387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>45190</v>
       </c>
@@ -14415,7 +14452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>45190</v>
       </c>
@@ -14480,7 +14517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>45190</v>
       </c>
@@ -14545,7 +14582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>45190</v>
       </c>
@@ -14610,7 +14647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>45220</v>
       </c>
@@ -14675,7 +14712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>45220</v>
       </c>
@@ -14740,7 +14777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>45220</v>
       </c>
@@ -14805,7 +14842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>45220</v>
       </c>
@@ -14870,7 +14907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>45220</v>
       </c>
@@ -14932,7 +14969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>45220</v>
       </c>
@@ -14997,7 +15034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>45220</v>
       </c>
@@ -15062,7 +15099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>45220</v>
       </c>
@@ -15127,7 +15164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>45220</v>
       </c>
@@ -15192,7 +15229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>45220</v>
       </c>
@@ -15257,7 +15294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>45251</v>
       </c>
@@ -15322,7 +15359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>45251</v>
       </c>
@@ -15387,7 +15424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>45251</v>
       </c>
@@ -15452,7 +15489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>45251</v>
       </c>
@@ -15517,7 +15554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>45251</v>
       </c>
@@ -15582,7 +15619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>45251</v>
       </c>
@@ -15647,7 +15684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>45251</v>
       </c>
@@ -15712,7 +15749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>45251</v>
       </c>
@@ -15774,7 +15811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>45251</v>
       </c>
@@ -15839,7 +15876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>45251</v>
       </c>
@@ -15904,7 +15941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>45281</v>
       </c>
@@ -15969,7 +16006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>45281</v>
       </c>
@@ -16034,7 +16071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>45281</v>
       </c>
@@ -16099,7 +16136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>45281</v>
       </c>
@@ -16161,7 +16198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>45281</v>
       </c>
@@ -16226,7 +16263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>45281</v>
       </c>
@@ -16291,7 +16328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>45281</v>
       </c>
@@ -16356,7 +16393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>45281</v>
       </c>
@@ -16421,7 +16458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>45281</v>
       </c>
@@ -16486,7 +16523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>45281</v>
       </c>
@@ -16551,7 +16588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -16613,7 +16650,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2021</v>
       </c>
@@ -16675,7 +16712,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2021</v>
       </c>
@@ -16737,7 +16774,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2021</v>
       </c>
@@ -16799,7 +16836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2021</v>
       </c>
@@ -16861,7 +16898,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2021</v>
       </c>
@@ -16923,7 +16960,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2021</v>
       </c>
@@ -16985,7 +17022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2021</v>
       </c>
@@ -17047,7 +17084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -17109,7 +17146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2021</v>
       </c>

</xml_diff>

<commit_message>
Health indicators visualizationpt.2 - JP
</commit_message>
<xml_diff>
--- a/data/July-Sep 2022/Reproductive maternal/Reproductive Health monthly prov.xlsx
+++ b/data/July-Sep 2022/Reproductive maternal/Reproductive Health monthly prov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JACK.PAYNE\Documents\Zambia-E4H\data\July-Sep 2022\Reproductive maternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DF5A23-68A1-48D4-9FB1-674E7C6E3718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AA5168-4D12-4980-AC7E-58D43A29BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7590" yWindow="430" windowWidth="15870" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reproductive Health Monthly dat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="61">
   <si>
     <t>periodname</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>anc_highrisk</t>
+  </si>
+  <si>
+    <t>deliv_staff</t>
+  </si>
+  <si>
+    <t>deliv</t>
+  </si>
+  <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>mat_dths_fac</t>
+  </si>
+  <si>
+    <t>fresh_still</t>
+  </si>
+  <si>
+    <t>pre_neo</t>
+  </si>
+  <si>
+    <t>still</t>
+  </si>
+  <si>
+    <t>mace_still</t>
   </si>
 </sst>
 </file>
@@ -8717,8 +8741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8830,31 +8854,31 @@
         <v>52</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>44</v>

</xml_diff>